<commit_message>
Add second table to sample files. Add import_tables function to backend.py which is information that will be needed to build the front end.
</commit_message>
<xml_diff>
--- a/samples/encounters.xlsx
+++ b/samples/encounters.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\random-encounter-generator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342249FD-A72A-4087-9999-42E0F2041F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78506D86-56A0-4661-930F-6EF9FEE99B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20070" yWindow="4785" windowWidth="19830" windowHeight="10680" xr2:uid="{D3490150-7E12-4C68-B688-AB47960AD7F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rolling Grasslands Tier3" sheetId="1" r:id="rId1"/>
+    <sheet name="Open Road Tier4" sheetId="2" r:id="rId1"/>
+    <sheet name="Rolling Grasslands Tier3" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
   <si>
     <t>D100</t>
   </si>
@@ -249,6 +250,105 @@
   </si>
   <si>
     <t>Malfunctioning planar portal</t>
+  </si>
+  <si>
+    <t>1–5</t>
+  </si>
+  <si>
+    <t>Arcane Blademaster</t>
+  </si>
+  <si>
+    <t>6–10</t>
+  </si>
+  <si>
+    <t>Archpriest</t>
+  </si>
+  <si>
+    <t>11–16</t>
+  </si>
+  <si>
+    <t>17–21</t>
+  </si>
+  <si>
+    <t>Ascetic Grandmaster</t>
+  </si>
+  <si>
+    <t>22–26</t>
+  </si>
+  <si>
+    <t>Dread Knight</t>
+  </si>
+  <si>
+    <t>27–31</t>
+  </si>
+  <si>
+    <t>Divine War</t>
+  </si>
+  <si>
+    <t>32–36</t>
+  </si>
+  <si>
+    <t>Empyrean</t>
+  </si>
+  <si>
+    <t>37–42</t>
+  </si>
+  <si>
+    <t>Hill Giant</t>
+  </si>
+  <si>
+    <t>43–47</t>
+  </si>
+  <si>
+    <t>God Corpse</t>
+  </si>
+  <si>
+    <t>48–53</t>
+  </si>
+  <si>
+    <t>55–60</t>
+  </si>
+  <si>
+    <t>61–65</t>
+  </si>
+  <si>
+    <t>Hallowed Ground</t>
+  </si>
+  <si>
+    <t>66–71</t>
+  </si>
+  <si>
+    <t>Master Assassin</t>
+  </si>
+  <si>
+    <t>Assassin</t>
+  </si>
+  <si>
+    <t>72–74</t>
+  </si>
+  <si>
+    <t>75-76</t>
+  </si>
+  <si>
+    <t>77–81</t>
+  </si>
+  <si>
+    <t>Killing Cloud</t>
+  </si>
+  <si>
+    <t>82–87</t>
+  </si>
+  <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>88–94</t>
+  </si>
+  <si>
+    <t>Wraith Lord</t>
+  </si>
+  <si>
+    <t>95–100</t>
   </si>
 </sst>
 </file>
@@ -633,10 +733,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9F2E29-4630-4A7F-8C44-A6CB1D6C6442}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA59092-17C8-46F5-9382-C0C8367C5D88}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B32" sqref="B32:C32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create functions, make_journey_window and make_journey_row, to generate the journey window for the users to pick type and tier of encounters and times of day to check. Update sample files, encounters.xlsx and tables.json, with better choices for starting adventures. Set defaults in the application to generate a simple seven-day hike to a village from a city.
</commit_message>
<xml_diff>
--- a/samples/encounters.xlsx
+++ b/samples/encounters.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\random-encounter-generator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78506D86-56A0-4661-930F-6EF9FEE99B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18B90CF1-1B3F-4E24-999F-2E0866DCBBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20070" yWindow="4785" windowWidth="19830" windowHeight="10680" xr2:uid="{D3490150-7E12-4C68-B688-AB47960AD7F2}"/>
+    <workbookView xWindow="-18375" yWindow="4830" windowWidth="19830" windowHeight="10680" activeTab="2" xr2:uid="{82D66F05-1E59-4819-8A3E-562F7EC1860F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Open Road Tier4" sheetId="2" r:id="rId1"/>
-    <sheet name="Rolling Grasslands Tier3" sheetId="1" r:id="rId2"/>
+    <sheet name="Country Shire Tier0" sheetId="1" r:id="rId1"/>
+    <sheet name="Open Roads Tier0" sheetId="2" r:id="rId2"/>
+    <sheet name="Urban Township Tier0" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="154">
   <si>
     <t>D100</t>
   </si>
@@ -48,37 +49,43 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t>1–3</t>
-  </si>
-  <si>
-    <t>Bridge of Sorrow</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Axe Beak</t>
+  </si>
+  <si>
+    <t>Mnst</t>
+  </si>
+  <si>
+    <t>2–3</t>
+  </si>
+  <si>
+    <t>Badger</t>
+  </si>
+  <si>
+    <t>4–5</t>
+  </si>
+  <si>
+    <t>Bridge of Stones</t>
   </si>
   <si>
     <t>Expl</t>
   </si>
   <si>
-    <t>4–6</t>
-  </si>
-  <si>
-    <t>Adult River Dragon</t>
-  </si>
-  <si>
-    <t>Mnst</t>
-  </si>
-  <si>
-    <t>7–9</t>
-  </si>
-  <si>
-    <t>Ankylosaurus</t>
-  </si>
-  <si>
-    <t>10–12</t>
-  </si>
-  <si>
-    <t>Blackguard</t>
-  </si>
-  <si>
-    <t>13–16</t>
+    <t>6–7</t>
+  </si>
+  <si>
+    <t>Bandit</t>
+  </si>
+  <si>
+    <t>8–9</t>
+  </si>
+  <si>
+    <t>Blink Dog</t>
+  </si>
+  <si>
+    <t>10–31</t>
   </si>
   <si>
     <t>Travel Scenery</t>
@@ -87,268 +94,412 @@
     <t>pg 105</t>
   </si>
   <si>
-    <t>17–19</t>
-  </si>
-  <si>
-    <t>Champion Warrior</t>
-  </si>
-  <si>
-    <t>20–22</t>
-  </si>
-  <si>
-    <t>Cyclops</t>
-  </si>
-  <si>
-    <t>23–25</t>
-  </si>
-  <si>
-    <t>Diplodocus</t>
-  </si>
-  <si>
-    <t>26–28</t>
-  </si>
-  <si>
-    <t>Caught in the Crossfire</t>
-  </si>
-  <si>
-    <t>29–31</t>
-  </si>
-  <si>
-    <t>Gorgon</t>
+    <t>32–33</t>
+  </si>
+  <si>
+    <t>Blood Hawk</t>
+  </si>
+  <si>
+    <t>34–35</t>
+  </si>
+  <si>
+    <t>Centaur</t>
+  </si>
+  <si>
+    <t>36–37</t>
+  </si>
+  <si>
+    <t>Deer</t>
+  </si>
+  <si>
+    <t>38–39</t>
+  </si>
+  <si>
+    <t>Enchanted Windmill</t>
+  </si>
+  <si>
+    <t>40–41</t>
+  </si>
+  <si>
+    <t>Druid</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Faerie Dragon</t>
+  </si>
+  <si>
+    <t>43–44</t>
+  </si>
+  <si>
+    <t>Giant Badger</t>
+  </si>
+  <si>
+    <t>45–46</t>
+  </si>
+  <si>
+    <t>End of Hibernation</t>
+  </si>
+  <si>
+    <t>47–48</t>
+  </si>
+  <si>
+    <t>Giant Poisonous Snake</t>
+  </si>
+  <si>
+    <t>49–50</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>51–52</t>
+  </si>
+  <si>
+    <t>Hawk</t>
+  </si>
+  <si>
+    <t>53–54</t>
+  </si>
+  <si>
+    <t>Forested Hills</t>
+  </si>
+  <si>
+    <t>55–56</t>
+  </si>
+  <si>
+    <t>Lizard</t>
+  </si>
+  <si>
+    <t>57–58</t>
+  </si>
+  <si>
+    <t>Noble</t>
+  </si>
+  <si>
+    <t>59–60</t>
+  </si>
+  <si>
+    <t>Hail Storm</t>
+  </si>
+  <si>
+    <t>61–63</t>
+  </si>
+  <si>
+    <t>Poisonous Snake</t>
+  </si>
+  <si>
+    <t>64–65</t>
+  </si>
+  <si>
+    <t>River Dragon Wyrmling</t>
+  </si>
+  <si>
+    <t>66–67</t>
+  </si>
+  <si>
+    <t>Haze</t>
+  </si>
+  <si>
+    <t>68–70</t>
+  </si>
+  <si>
+    <t>Scarecrow</t>
+  </si>
+  <si>
+    <t>71–72</t>
+  </si>
+  <si>
+    <t>Scout</t>
+  </si>
+  <si>
+    <t>73–74</t>
+  </si>
+  <si>
+    <t>Lost Item</t>
+  </si>
+  <si>
+    <t>75–76</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>77–80</t>
+  </si>
+  <si>
+    <t>Public Ceremony</t>
+  </si>
+  <si>
+    <t>81–82</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>83–84</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>85–99</t>
+  </si>
+  <si>
+    <t>Social Encounter</t>
+  </si>
+  <si>
+    <t>pg 103</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Mushroom Ring</t>
+  </si>
+  <si>
+    <t>Awakened Shrub</t>
+  </si>
+  <si>
+    <t>Counterfeit Goods</t>
+  </si>
+  <si>
+    <t>Cockatrice</t>
+  </si>
+  <si>
+    <t>Cult Fanatic</t>
+  </si>
+  <si>
+    <t>10–19</t>
+  </si>
+  <si>
+    <t>20–21</t>
+  </si>
+  <si>
+    <t>Cultist</t>
+  </si>
+  <si>
+    <t>22–23</t>
+  </si>
+  <si>
+    <t>Ettercap</t>
+  </si>
+  <si>
+    <t>24–25</t>
+  </si>
+  <si>
+    <t>26–27</t>
+  </si>
+  <si>
+    <t>Ghoul</t>
+  </si>
+  <si>
+    <t>28–29</t>
+  </si>
+  <si>
+    <t>Giant Spider</t>
+  </si>
+  <si>
+    <t>30–31</t>
   </si>
   <si>
     <t>32–34</t>
   </si>
   <si>
-    <t>Harpy</t>
+    <t>Giant Wolf Spider</t>
   </si>
   <si>
     <t>35–37</t>
   </si>
   <si>
-    <t>Hobgoblin Warlord</t>
-  </si>
-  <si>
-    <t>38–39</t>
-  </si>
-  <si>
-    <t>Choking Smoke</t>
-  </si>
-  <si>
-    <t>40–45</t>
-  </si>
-  <si>
-    <t>Holy Knight</t>
+    <t>38–41</t>
+  </si>
+  <si>
+    <t>Falling Net</t>
+  </si>
+  <si>
+    <t>Kobold</t>
+  </si>
+  <si>
+    <t>43–45</t>
   </si>
   <si>
     <t>46–48</t>
   </si>
   <si>
-    <t>Invisible Stalker</t>
-  </si>
-  <si>
     <t>49–51</t>
   </si>
   <si>
-    <t>Knight Captain</t>
+    <t>Ogre Zombie</t>
   </si>
   <si>
     <t>52–54</t>
   </si>
   <si>
-    <t>Cursed Waterway</t>
-  </si>
-  <si>
     <t>55–57</t>
   </si>
   <si>
-    <t>Ogre Mage</t>
-  </si>
-  <si>
-    <t>58–61</t>
-  </si>
-  <si>
-    <t>Rakshasa</t>
-  </si>
-  <si>
-    <t>62–64</t>
-  </si>
-  <si>
-    <t>Roc</t>
-  </si>
-  <si>
-    <t>65–69</t>
-  </si>
-  <si>
-    <t>Endless Plummet</t>
-  </si>
-  <si>
-    <t>70–73</t>
-  </si>
-  <si>
-    <t>Soldier Squad</t>
-  </si>
-  <si>
-    <t>74–76</t>
-  </si>
-  <si>
-    <t>Triceratops</t>
-  </si>
-  <si>
-    <t>77–78</t>
-  </si>
-  <si>
-    <t>Troll</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>Dread Troll</t>
-  </si>
-  <si>
-    <t>80–82</t>
-  </si>
-  <si>
-    <t>Fey Glade</t>
-  </si>
-  <si>
-    <t>83–85</t>
-  </si>
-  <si>
-    <t>Tyrannosaurus Rex</t>
-  </si>
-  <si>
-    <t>86–88</t>
-  </si>
-  <si>
-    <t>Weretiger</t>
-  </si>
-  <si>
-    <t>89–90</t>
-  </si>
-  <si>
-    <t>Wyvern</t>
-  </si>
-  <si>
-    <t>91–92</t>
-  </si>
-  <si>
-    <t>Sunspots</t>
-  </si>
-  <si>
-    <t>93–99</t>
-  </si>
-  <si>
-    <t>Social Encounter</t>
-  </si>
-  <si>
-    <t>pg 103</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Malfunctioning planar portal</t>
-  </si>
-  <si>
-    <t>1–5</t>
-  </si>
-  <si>
-    <t>Arcane Blademaster</t>
-  </si>
-  <si>
-    <t>6–10</t>
-  </si>
-  <si>
-    <t>Archpriest</t>
-  </si>
-  <si>
-    <t>11–16</t>
-  </si>
-  <si>
-    <t>17–21</t>
-  </si>
-  <si>
-    <t>Ascetic Grandmaster</t>
-  </si>
-  <si>
-    <t>22–26</t>
-  </si>
-  <si>
-    <t>Dread Knight</t>
-  </si>
-  <si>
-    <t>27–31</t>
-  </si>
-  <si>
-    <t>Divine War</t>
-  </si>
-  <si>
-    <t>32–36</t>
-  </si>
-  <si>
-    <t>Empyrean</t>
-  </si>
-  <si>
-    <t>37–42</t>
-  </si>
-  <si>
-    <t>Hill Giant</t>
-  </si>
-  <si>
-    <t>43–47</t>
-  </si>
-  <si>
-    <t>God Corpse</t>
-  </si>
-  <si>
-    <t>48–53</t>
-  </si>
-  <si>
-    <t>55–60</t>
-  </si>
-  <si>
-    <t>61–65</t>
-  </si>
-  <si>
-    <t>Hallowed Ground</t>
-  </si>
-  <si>
-    <t>66–71</t>
-  </si>
-  <si>
-    <t>Master Assassin</t>
-  </si>
-  <si>
-    <t>Assassin</t>
-  </si>
-  <si>
-    <t>72–74</t>
-  </si>
-  <si>
-    <t>75-76</t>
-  </si>
-  <si>
-    <t>77–81</t>
-  </si>
-  <si>
-    <t>Killing Cloud</t>
-  </si>
-  <si>
-    <t>82–87</t>
-  </si>
-  <si>
-    <t>Vampire</t>
-  </si>
-  <si>
-    <t>88–94</t>
-  </si>
-  <si>
-    <t>Wraith Lord</t>
-  </si>
-  <si>
-    <t>95–100</t>
+    <t>58–60</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Skeleton</t>
+  </si>
+  <si>
+    <t>64–66</t>
+  </si>
+  <si>
+    <t>Landslide</t>
+  </si>
+  <si>
+    <t>67–69</t>
+  </si>
+  <si>
+    <t>Specter</t>
+  </si>
+  <si>
+    <t>70–71</t>
+  </si>
+  <si>
+    <t>Swarm</t>
+  </si>
+  <si>
+    <t>72–73</t>
+  </si>
+  <si>
+    <t>74–75</t>
+  </si>
+  <si>
+    <t>Wererat</t>
+  </si>
+  <si>
+    <t>76–77</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>78–79</t>
+  </si>
+  <si>
+    <t>80–99</t>
+  </si>
+  <si>
+    <t>Pests</t>
+  </si>
+  <si>
+    <t>Aboleth Thrall</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Acolyte</t>
+  </si>
+  <si>
+    <t>3–4</t>
+  </si>
+  <si>
+    <t>Apprentice Mage</t>
+  </si>
+  <si>
+    <t>5–6</t>
+  </si>
+  <si>
+    <t>7–8</t>
+  </si>
+  <si>
+    <t>9–10</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>11–12</t>
+  </si>
+  <si>
+    <t>Commoner</t>
+  </si>
+  <si>
+    <t>13–25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27–28</t>
+  </si>
+  <si>
+    <t>29–30</t>
+  </si>
+  <si>
+    <t>Cutthroat</t>
+  </si>
+  <si>
+    <t>31–32</t>
+  </si>
+  <si>
+    <t>33–34</t>
+  </si>
+  <si>
+    <t>Gargoyle</t>
+  </si>
+  <si>
+    <t>35–36</t>
+  </si>
+  <si>
+    <t>Giant Rat</t>
+  </si>
+  <si>
+    <t>37–40</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>41–42</t>
+  </si>
+  <si>
+    <t>Imp</t>
+  </si>
+  <si>
+    <t>Mastiff</t>
+  </si>
+  <si>
+    <t>Minstrel</t>
+  </si>
+  <si>
+    <t>Spy (Cutthroat Variant)</t>
+  </si>
+  <si>
+    <t>Steam Mephit</t>
+  </si>
+  <si>
+    <t>61–62</t>
+  </si>
+  <si>
+    <t>Swarm of Rats</t>
+  </si>
+  <si>
+    <t>63–64</t>
+  </si>
+  <si>
+    <t>Thug</t>
+  </si>
+  <si>
+    <t>65–66</t>
+  </si>
+  <si>
+    <t>67–68</t>
+  </si>
+  <si>
+    <t>69–99</t>
+  </si>
+  <si>
+    <t>Dark Alleys</t>
   </si>
 </sst>
 </file>
@@ -733,16 +884,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9F2E29-4630-4A7F-8C44-A6CB1D6C6442}">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA2127E-4F74-422E-8713-D5A0378E1130}">
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,99 +908,99 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>71</v>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -857,32 +1008,32 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>90</v>
+      <c r="A13" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
@@ -890,43 +1041,43 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>96</v>
+      <c r="A16" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
@@ -934,35 +1085,189 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>68</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -972,16 +1277,398 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA59092-17C8-46F5-9382-C0C8367C5D88}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6575DB49-9F30-4B13-A843-7CFD0ED9C8E4}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E7490F-3028-414C-8900-04E3932D2F77}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B32" sqref="B32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -996,99 +1683,99 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
+      <c r="A10" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1096,43 +1783,43 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>5</v>
@@ -1140,43 +1827,43 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
@@ -1184,43 +1871,43 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
@@ -1228,54 +1915,54 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>54</v>
+      <c r="A26" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -1283,68 +1970,57 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>151</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>152</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>66</v>
+      <c r="A32" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>